<commit_message>
adjusted position of the filename in the pdf script
</commit_message>
<xml_diff>
--- a/excel/linksco.xlsx
+++ b/excel/linksco.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankur.chadha\Desktop\Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankur.chadha\Desktop\GrizzlyClone\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D7587B-82ED-4DE4-B1DE-39151FCDD892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F3A937-9733-47E2-9DF9-8067496F31C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABD09717-DAD3-4D53-9B45-E0E333E575C0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABD09717-DAD3-4D53-9B45-E0E333E575C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -218,12 +218,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -239,12 +245,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -563,7 +570,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +721,7 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="5" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>